<commit_message>
Atualização para versão 1.1 com melhorias estatísticas
</commit_message>
<xml_diff>
--- a/dados/resultados_euromilhoes.xlsx
+++ b/dados/resultados_euromilhoes.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\PyCharmMiscProject\euromilhoes_app\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C36FB8-C3CA-492D-A6A9-C106A07E3EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F229048-743A-4DEA-A06A-25CF9C4FE0E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arquivo de resultados" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Arquivo de resultados'!$A$2:$J$1858</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Arquivo de resultados'!$A$2:$J$1859</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1863" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1864" uniqueCount="8">
   <si>
     <t>Arquivo</t>
   </si>
@@ -532,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U1859"/>
+  <dimension ref="A1:U1860"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1828" workbookViewId="0">
-      <selection activeCell="G1859" sqref="G1859"/>
+    <sheetView tabSelected="1" topLeftCell="A1846" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A1861" sqref="A1861"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60036,6 +60036,38 @@
         <v>5</v>
       </c>
     </row>
+    <row r="1860" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1860" s="2">
+        <v>45849</v>
+      </c>
+      <c r="B1860" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1860" s="8">
+        <v>1858</v>
+      </c>
+      <c r="D1860" s="8">
+        <v>8</v>
+      </c>
+      <c r="E1860" s="8">
+        <v>23</v>
+      </c>
+      <c r="F1860" s="8">
+        <v>24</v>
+      </c>
+      <c r="G1860" s="8">
+        <v>45</v>
+      </c>
+      <c r="H1860" s="8">
+        <v>49</v>
+      </c>
+      <c r="I1860" s="8">
+        <v>2</v>
+      </c>
+      <c r="J1860" s="8">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>

</xml_diff>

<commit_message>
Sobrescrita dos ficheiros Python para v1.2
</commit_message>
<xml_diff>
--- a/dados/resultados_euromilhoes.xlsx
+++ b/dados/resultados_euromilhoes.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\PyCharmMiscProject\euromilhoes_app\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F229048-743A-4DEA-A06A-25CF9C4FE0E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C5E80A-E5A6-4472-BAEF-CC9043455B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="8100" windowWidth="14610" windowHeight="8205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arquivo de resultados" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Arquivo de resultados'!$A$2:$J$1859</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Arquivo de resultados'!$A$2:$J$1860</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U1860"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1846" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A1861" sqref="A1861"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60069,6 +60069,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:J1860" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>

</xml_diff>

<commit_message>
✨ Substituídos ficheiros do projeto pela versão oficial v1.3 — atualização completa
</commit_message>
<xml_diff>
--- a/dados/resultados_euromilhoes.xlsx
+++ b/dados/resultados_euromilhoes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\PyCharmMiscProject\euromilhoes_app\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C5E80A-E5A6-4472-BAEF-CC9043455B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823C5174-C7D5-41BB-AF10-B42C7C9163CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="8100" windowWidth="14610" windowHeight="8205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arquivo de resultados" sheetId="1" r:id="rId1"/>

</xml_diff>